<commit_message>
update inline release names, bugs fixes
</commit_message>
<xml_diff>
--- a/release-notes/2022-11/closed-bugs-sle-2022-11.xlsx
+++ b/release-notes/2022-11/closed-bugs-sle-2022-11.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markblack/repos/github/install-systemlink-enterprise/release-notes/11-2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markblack/repos/github/install-systemlink-enterprise/release-notes/2022-11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDEDFC6-2201-A245-BB37-FDB6E3798424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489CF0C7-D222-0D40-847F-0E20F8E6D999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Update RabbitMQ Helm Chart</t>
   </si>
   <si>
-    <t xml:space="preserve">[XRAY - nbparsingservice, nbexecworker, jupyter-notebook-userpod] Make base image tag more specific </t>
-  </si>
-  <si>
     <t>All SLE users can see policies IDs and entitlements for all other users in the same org</t>
   </si>
   <si>
@@ -122,6 +119,12 @@
   </si>
   <si>
     <t>Need to support Group by Hidden Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[XRAY] nbparsingservice, nbexecworker, jupyter-notebook-userpod - Make base image tag more specific </t>
+  </si>
+  <si>
+    <t>[XRAY] "system.drawing.common" package on .NET builds</t>
   </si>
 </sst>
 </file>
@@ -605,8 +608,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -962,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F31" sqref="F31:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1038,7 +1042,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -1136,7 +1140,7 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
@@ -1164,7 +1168,7 @@
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
@@ -1198,7 +1202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2167479</v>
       </c>
@@ -1212,7 +1216,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2119196</v>
       </c>
@@ -1226,7 +1230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2145644</v>
       </c>
@@ -1240,7 +1244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2192619</v>
       </c>
@@ -1254,7 +1258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2181700</v>
       </c>
@@ -1268,7 +1272,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2047675</v>
       </c>
@@ -1282,7 +1286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2159327</v>
       </c>
@@ -1296,9 +1300,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>2156702</v>
+        <v>2171852</v>
       </c>
       <c r="B24" t="s">
         <v>4</v>
@@ -1310,9 +1314,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2171852</v>
+        <v>2193592</v>
       </c>
       <c r="B25" t="s">
         <v>4</v>
@@ -1324,9 +1328,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2193592</v>
+        <v>2193582</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
@@ -1338,9 +1342,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>2193582</v>
+        <v>2193574</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
@@ -1352,9 +1356,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>2193574</v>
+        <v>2193554</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
@@ -1366,47 +1370,63 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>2193554</v>
+        <v>2181700</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>2181700</v>
+        <v>2171177</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>2171177</v>
+        <v>2203752</v>
       </c>
       <c r="B31" t="s">
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2156702</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>